<commit_message>
glider 376 recovered - entered date
Cal sheet update : entered the recovery date of glider 376 - 2016-08-09
09:15 UTC
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP05MOAS-GL376_00005.xlsx
+++ b/deployment/Omaha_Cal_Info_CP05MOAS-GL376_00005.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leila/Documents/OOI_assmgt/asset-management/deployment/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6440" yWindow="5640" windowWidth="23460" windowHeight="10240" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="540" yWindow="3260" windowWidth="23460" windowHeight="10240" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -32,6 +37,9 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -40,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
   <si>
     <t>Ref Des</t>
   </si>
@@ -201,7 +209,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -320,6 +328,11 @@
       <color rgb="FF484848"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
     </font>
   </fonts>
   <fills count="4">
@@ -426,7 +439,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -503,6 +516,7 @@
     <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="32">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -908,11 +922,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
@@ -923,7 +937,7 @@
     <col min="12" max="12" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="28">
+    <row r="1" spans="1:14" ht="28" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
         <v>34</v>
       </c>
@@ -961,7 +975,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="24" customFormat="1" ht="15">
+    <row r="2" spans="1:14" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -980,8 +994,8 @@
       <c r="F2" s="5">
         <v>0.86805555555555547</v>
       </c>
-      <c r="G2" s="29" t="s">
-        <v>44</v>
+      <c r="G2" s="32">
+        <v>42591</v>
       </c>
       <c r="H2" s="22" t="s">
         <v>45</v>
@@ -1005,67 +1019,62 @@
         <v>-70.533333330000005</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G7" s="28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15">
+    <row r="12" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
     </row>
-    <row r="13" spans="1:14" ht="15">
+    <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="8:9">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="8:9">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="8:9">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="8:9">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="8:9">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.2">
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1073,11 +1082,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.5" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
@@ -1089,7 +1098,7 @@
     <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="28">
+    <row r="1" spans="1:19" ht="28" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -1115,7 +1124,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
@@ -1154,7 +1163,7 @@
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
@@ -1193,7 +1202,7 @@
       <c r="R3" s="12"/>
       <c r="S3" s="12"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -1232,7 +1241,7 @@
       <c r="R4" s="12"/>
       <c r="S4" s="12"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -1271,7 +1280,7 @@
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="9"/>
@@ -1292,7 +1301,7 @@
       <c r="R6" s="12"/>
       <c r="S6" s="12"/>
     </row>
-    <row r="7" spans="1:19" s="2" customFormat="1">
+    <row r="7" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>29</v>
       </c>
@@ -1326,7 +1335,7 @@
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
     </row>
-    <row r="8" spans="1:19" s="2" customFormat="1">
+    <row r="8" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>29</v>
       </c>
@@ -1360,7 +1369,7 @@
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
     </row>
-    <row r="9" spans="1:19" s="2" customFormat="1">
+    <row r="9" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
@@ -1394,7 +1403,7 @@
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
     </row>
-    <row r="10" spans="1:19" s="2" customFormat="1">
+    <row r="10" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
@@ -1428,7 +1437,7 @@
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
     </row>
-    <row r="11" spans="1:19" s="2" customFormat="1">
+    <row r="11" spans="1:19" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="9"/>
@@ -1444,7 +1453,7 @@
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
     </row>
-    <row r="12" spans="1:19" s="2" customFormat="1">
+    <row r="12" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>30</v>
       </c>
@@ -1474,7 +1483,7 @@
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
     </row>
-    <row r="13" spans="1:19" s="2" customFormat="1">
+    <row r="13" spans="1:19" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="9"/>
@@ -1492,7 +1501,7 @@
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
     </row>
-    <row r="14" spans="1:19" s="2" customFormat="1">
+    <row r="14" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>31</v>
       </c>
@@ -1522,7 +1531,7 @@
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
     </row>
-    <row r="15" spans="1:19" s="2" customFormat="1">
+    <row r="15" spans="1:19" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="9"/>
@@ -1538,7 +1547,7 @@
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
     </row>
-    <row r="16" spans="1:19" s="2" customFormat="1">
+    <row r="16" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>32</v>
       </c>
@@ -1570,7 +1579,7 @@
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
     </row>
-    <row r="17" spans="1:14" s="2" customFormat="1">
+    <row r="17" spans="1:14" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="9"/>
@@ -1586,7 +1595,7 @@
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
     </row>
-    <row r="18" spans="1:14" s="2" customFormat="1">
+    <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>33</v>
       </c>
@@ -1616,7 +1625,7 @@
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
     </row>
-    <row r="19" spans="1:14" s="2" customFormat="1">
+    <row r="19" spans="1:14" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="9"/>
@@ -1632,13 +1641,13 @@
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
@@ -1647,10 +1656,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>